<commit_message>
fixed up lockdown dates data and added documentation
</commit_message>
<xml_diff>
--- a/data-raw/LockdownData.xlsx
+++ b/data-raw/LockdownData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joannawalsh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joannawalsh/Desktop/RforHDSdata/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45506852-7258-2F40-9132-C3D5E37345B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A32728-DE9D-8A4C-8A3A-C8EDF02C29EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="6140" windowWidth="27640" windowHeight="16940" xr2:uid="{F4A975AD-E28F-1045-BBFF-579E54AC5F04}"/>
+    <workbookView xWindow="5820" yWindow="760" windowWidth="27640" windowHeight="16940" xr2:uid="{F4A975AD-E28F-1045-BBFF-579E54AC5F04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -204,6 +204,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -235,7 +238,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777C5B6F-42BD-154A-B255-D41D44E7900B}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>